<commit_message>
Improved fit model, exporting outputs, and others
</commit_message>
<xml_diff>
--- a/data/calibration.xlsx
+++ b/data/calibration.xlsx
@@ -1,27 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aschwalbc/Documents/Research/ACF-VN/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CBE0C0-8652-864E-B47F-31320821C7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B41DB6E-D1DB-1B48-8363-C0CA018117AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16600" yWindow="860" windowWidth="16600" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37900" yWindow="500" windowWidth="37900" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notifications" sheetId="1" r:id="rId1"/>
     <sheet name="mortality" sheetId="2" r:id="rId2"/>
-    <sheet name="prevalence" sheetId="3" r:id="rId3"/>
-    <sheet name="incidence" sheetId="4" r:id="rId4"/>
-    <sheet name="demography" sheetId="5" r:id="rId5"/>
-    <sheet name="setting" sheetId="6" r:id="rId6"/>
-    <sheet name="sep" sheetId="7" r:id="rId7"/>
-    <sheet name="drug_sensitivity" sheetId="8" r:id="rId8"/>
-    <sheet name="hiv_status" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="42">
   <si>
     <t>variable_name</t>
   </si>
@@ -148,73 +141,25 @@
     <t>From 'WHO TB burden estimates [0.8Mb]' in https://www.who.int/teams/global-tuberculosis-programme/data</t>
   </si>
   <si>
-    <t>e_inc_num</t>
+    <t>pop (&gt;=15yo)</t>
   </si>
   <si>
-    <t>Estimated number of incident cases (all forms)</t>
+    <t>val</t>
   </si>
   <si>
-    <t>e_inc_num_lo</t>
+    <t>lo</t>
   </si>
   <si>
-    <t>Estimated number of incident cases (all forms), high bound</t>
+    <t>hi</t>
   </si>
   <si>
-    <t>e_inc_num_hi</t>
+    <t>mortrate per 100k</t>
   </si>
   <si>
-    <t>Estimated number of incident cases (all forms), low bound</t>
+    <t>all pop</t>
   </si>
   <si>
-    <t>MDR-TB rate among new cases (%)</t>
-  </si>
-  <si>
-    <t>MDR-TB rate among previously treated cases (%)</t>
-  </si>
-  <si>
-    <t>From 'The fourth national anti-tuberculosis drug resistance survey in Viet Nam'</t>
-  </si>
-  <si>
-    <t>estimate</t>
-  </si>
-  <si>
-    <t>Estimated adults and children living with HIV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">low </t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>Adults (15-49) prevalence (%)</t>
-  </si>
-  <si>
-    <t>From https://www.unaids.org/en/resources/documents/2021/HIV_estimates_with_uncertainty_bounds_1990-present</t>
-  </si>
-  <si>
-    <t>total population (8911)</t>
-  </si>
-  <si>
-    <t>total population (8921)</t>
-  </si>
-  <si>
-    <t>total population (8931)</t>
-  </si>
-  <si>
-    <t>https://population.un.org/wpp/Download/Files/1_Indicators%20(Standard)/EXCEL_FILES/2_Population/WPP2022_POP_F02_1_POPULATION_5-YEAR_AGE_GROUPS_BOTH_SEXES.xlsx</t>
-  </si>
-  <si>
-    <t>rate</t>
-  </si>
-  <si>
-    <t>per 100,000</t>
-  </si>
-  <si>
-    <t>mortrate</t>
-  </si>
-  <si>
-    <t>total population (&gt;=15 yo)</t>
+    <t>notifications per 100k</t>
   </si>
 </sst>
 </file>
@@ -224,7 +169,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -273,12 +218,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF1155CC"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -306,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -318,9 +257,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,18 +477,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA998"/>
+  <dimension ref="A1:AA993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="211" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1244,21 +1183,19 @@
       <c r="AA20" s="1"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>54</v>
+      <c r="A21" s="7"/>
+      <c r="C21" s="8" t="s">
+        <v>35</v>
       </c>
-      <c r="B21" s="1">
-        <v>2020</v>
+      <c r="D21" s="8" t="s">
+        <v>36</v>
       </c>
-      <c r="C21" s="10">
-        <f>C2/demography!C4*100000</f>
-        <v>73.151800498594142</v>
+      <c r="E21" s="8" t="s">
+        <v>37</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>55</v>
+      <c r="F21" s="8" t="s">
+        <v>38</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1282,21 +1219,27 @@
       <c r="AA21" s="1"/>
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
-        <v>54</v>
+      <c r="A22" s="8" t="s">
+        <v>41</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>2010</v>
       </c>
-      <c r="C22" s="10">
-        <f>C7/demography!C3*100000</f>
+      <c r="C22">
+        <v>65662656</v>
+      </c>
+      <c r="D22" s="10">
+        <f>C7/C22*100000</f>
         <v>79.413479710598367</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>55</v>
+      <c r="E22" s="9">
+        <f>D22-(2*(D22*0.1))</f>
+        <v>63.530783768478692</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="9">
+        <f>D22+(2*(D22*0.1))</f>
+        <v>95.296175652718034</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1320,12 +1263,27 @@
       <c r="AA22" s="1"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="A23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23">
+        <v>2020</v>
+      </c>
+      <c r="C23">
+        <v>74292088</v>
+      </c>
+      <c r="D23" s="10">
+        <f>C2/C23*100000</f>
+        <v>73.151800498594142</v>
+      </c>
+      <c r="E23" s="9">
+        <f>D23-(2*(D23*0.1))</f>
+        <v>58.521440398875313</v>
+      </c>
+      <c r="F23" s="9">
+        <f>D23+(2*(D23*0.1))</f>
+        <v>87.78216059831297</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1349,12 +1307,6 @@
       <c r="AA23" s="1"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1378,12 +1330,19 @@
       <c r="AA24" s="1"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="A25" s="7"/>
+      <c r="C25" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1407,12 +1366,27 @@
       <c r="AA25" s="1"/>
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="A26" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26">
+        <v>2010</v>
+      </c>
+      <c r="C26">
+        <v>86944961</v>
+      </c>
+      <c r="D26" s="10">
+        <f>C7/C26*100000</f>
+        <v>59.974723549533827</v>
+      </c>
+      <c r="E26" s="9">
+        <f>D26-(2*(D26*0.1))</f>
+        <v>47.979778839627059</v>
+      </c>
+      <c r="F26" s="9">
+        <f>D26+(2*(D26*0.1))</f>
+        <v>71.969668259440596</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -1436,12 +1410,27 @@
       <c r="AA26" s="1"/>
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="A27" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27">
+        <v>2020</v>
+      </c>
+      <c r="C27">
+        <v>96203595</v>
+      </c>
+      <c r="D27" s="10">
+        <f>C2/C27*100000</f>
+        <v>56.490612435013468</v>
+      </c>
+      <c r="E27" s="9">
+        <f>D27-(2*(D27*0.1))</f>
+        <v>45.192489948010774</v>
+      </c>
+      <c r="F27" s="9">
+        <f>D27+(2*(D27*0.1))</f>
+        <v>67.788734922016161</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -2305,7 +2294,7 @@
       <c r="Z56" s="1"/>
       <c r="AA56" s="1"/>
     </row>
-    <row r="57" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2334,7 +2323,7 @@
       <c r="Z57" s="1"/>
       <c r="AA57" s="1"/>
     </row>
-    <row r="58" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2363,7 +2352,7 @@
       <c r="Z58" s="1"/>
       <c r="AA58" s="1"/>
     </row>
-    <row r="59" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2392,7 +2381,7 @@
       <c r="Z59" s="1"/>
       <c r="AA59" s="1"/>
     </row>
-    <row r="60" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2421,7 +2410,7 @@
       <c r="Z60" s="1"/>
       <c r="AA60" s="1"/>
     </row>
-    <row r="61" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -29478,151 +29467,6 @@
       <c r="Z993" s="1"/>
       <c r="AA993" s="1"/>
     </row>
-    <row r="994" spans="1:27" ht="13" x14ac:dyDescent="0.15">
-      <c r="A994" s="1"/>
-      <c r="B994" s="1"/>
-      <c r="C994" s="1"/>
-      <c r="D994" s="1"/>
-      <c r="E994" s="1"/>
-      <c r="F994" s="1"/>
-      <c r="G994" s="1"/>
-      <c r="H994" s="1"/>
-      <c r="I994" s="1"/>
-      <c r="J994" s="1"/>
-      <c r="K994" s="1"/>
-      <c r="L994" s="1"/>
-      <c r="M994" s="1"/>
-      <c r="N994" s="1"/>
-      <c r="O994" s="1"/>
-      <c r="P994" s="1"/>
-      <c r="Q994" s="1"/>
-      <c r="R994" s="1"/>
-      <c r="S994" s="1"/>
-      <c r="T994" s="1"/>
-      <c r="U994" s="1"/>
-      <c r="V994" s="1"/>
-      <c r="W994" s="1"/>
-      <c r="X994" s="1"/>
-      <c r="Y994" s="1"/>
-      <c r="Z994" s="1"/>
-      <c r="AA994" s="1"/>
-    </row>
-    <row r="995" spans="1:27" ht="13" x14ac:dyDescent="0.15">
-      <c r="A995" s="1"/>
-      <c r="B995" s="1"/>
-      <c r="C995" s="1"/>
-      <c r="D995" s="1"/>
-      <c r="E995" s="1"/>
-      <c r="F995" s="1"/>
-      <c r="G995" s="1"/>
-      <c r="H995" s="1"/>
-      <c r="I995" s="1"/>
-      <c r="J995" s="1"/>
-      <c r="K995" s="1"/>
-      <c r="L995" s="1"/>
-      <c r="M995" s="1"/>
-      <c r="N995" s="1"/>
-      <c r="O995" s="1"/>
-      <c r="P995" s="1"/>
-      <c r="Q995" s="1"/>
-      <c r="R995" s="1"/>
-      <c r="S995" s="1"/>
-      <c r="T995" s="1"/>
-      <c r="U995" s="1"/>
-      <c r="V995" s="1"/>
-      <c r="W995" s="1"/>
-      <c r="X995" s="1"/>
-      <c r="Y995" s="1"/>
-      <c r="Z995" s="1"/>
-      <c r="AA995" s="1"/>
-    </row>
-    <row r="996" spans="1:27" ht="13" x14ac:dyDescent="0.15">
-      <c r="A996" s="1"/>
-      <c r="B996" s="1"/>
-      <c r="C996" s="1"/>
-      <c r="D996" s="1"/>
-      <c r="E996" s="1"/>
-      <c r="F996" s="1"/>
-      <c r="G996" s="1"/>
-      <c r="H996" s="1"/>
-      <c r="I996" s="1"/>
-      <c r="J996" s="1"/>
-      <c r="K996" s="1"/>
-      <c r="L996" s="1"/>
-      <c r="M996" s="1"/>
-      <c r="N996" s="1"/>
-      <c r="O996" s="1"/>
-      <c r="P996" s="1"/>
-      <c r="Q996" s="1"/>
-      <c r="R996" s="1"/>
-      <c r="S996" s="1"/>
-      <c r="T996" s="1"/>
-      <c r="U996" s="1"/>
-      <c r="V996" s="1"/>
-      <c r="W996" s="1"/>
-      <c r="X996" s="1"/>
-      <c r="Y996" s="1"/>
-      <c r="Z996" s="1"/>
-      <c r="AA996" s="1"/>
-    </row>
-    <row r="997" spans="1:27" ht="13" x14ac:dyDescent="0.15">
-      <c r="A997" s="1"/>
-      <c r="B997" s="1"/>
-      <c r="C997" s="1"/>
-      <c r="D997" s="1"/>
-      <c r="E997" s="1"/>
-      <c r="F997" s="1"/>
-      <c r="G997" s="1"/>
-      <c r="H997" s="1"/>
-      <c r="I997" s="1"/>
-      <c r="J997" s="1"/>
-      <c r="K997" s="1"/>
-      <c r="L997" s="1"/>
-      <c r="M997" s="1"/>
-      <c r="N997" s="1"/>
-      <c r="O997" s="1"/>
-      <c r="P997" s="1"/>
-      <c r="Q997" s="1"/>
-      <c r="R997" s="1"/>
-      <c r="S997" s="1"/>
-      <c r="T997" s="1"/>
-      <c r="U997" s="1"/>
-      <c r="V997" s="1"/>
-      <c r="W997" s="1"/>
-      <c r="X997" s="1"/>
-      <c r="Y997" s="1"/>
-      <c r="Z997" s="1"/>
-      <c r="AA997" s="1"/>
-    </row>
-    <row r="998" spans="1:27" ht="13" x14ac:dyDescent="0.15">
-      <c r="A998" s="1"/>
-      <c r="B998" s="1"/>
-      <c r="C998" s="1"/>
-      <c r="D998" s="1"/>
-      <c r="E998" s="1"/>
-      <c r="F998" s="1"/>
-      <c r="G998" s="1"/>
-      <c r="H998" s="1"/>
-      <c r="I998" s="1"/>
-      <c r="J998" s="1"/>
-      <c r="K998" s="1"/>
-      <c r="L998" s="1"/>
-      <c r="M998" s="1"/>
-      <c r="N998" s="1"/>
-      <c r="O998" s="1"/>
-      <c r="P998" s="1"/>
-      <c r="Q998" s="1"/>
-      <c r="R998" s="1"/>
-      <c r="S998" s="1"/>
-      <c r="T998" s="1"/>
-      <c r="U998" s="1"/>
-      <c r="V998" s="1"/>
-      <c r="W998" s="1"/>
-      <c r="X998" s="1"/>
-      <c r="Y998" s="1"/>
-      <c r="Z998" s="1"/>
-      <c r="AA998" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29633,10 +29477,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="F40" sqref="A32:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -29869,7 +29713,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>28</v>
       </c>
@@ -29883,7 +29727,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>30</v>
       </c>
@@ -29897,7 +29741,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -29911,7 +29755,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
@@ -29925,7 +29769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
@@ -29939,7 +29783,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
@@ -29953,7 +29797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -29967,7 +29811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
         <v>24</v>
       </c>
@@ -29981,7 +29825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
@@ -29995,7 +29839,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
@@ -30009,7 +29853,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
         <v>30</v>
       </c>
@@ -30023,7 +29867,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
         <v>32</v>
       </c>
@@ -30037,57 +29881,180 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="9" t="s">
-        <v>56</v>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="7"/>
+      <c r="C32" s="8" t="s">
+        <v>35</v>
       </c>
-      <c r="B32">
+      <c r="D32" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33">
         <v>2000</v>
       </c>
-      <c r="C32" s="11">
-        <f>C23/demography!C2*100000</f>
+      <c r="C33">
+        <v>53576592</v>
+      </c>
+      <c r="D33" s="10">
+        <f>C23/C33*100000</f>
         <v>59.727576550595082</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>55</v>
+      <c r="E33" s="9">
+        <f>C25/C33*100000</f>
+        <v>37.329735344121922</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="9" t="s">
-        <v>56</v>
+      <c r="F33" s="9">
+        <f>C24/C33*100000</f>
+        <v>87.724878058686528</v>
       </c>
-      <c r="B33">
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34">
         <v>2010</v>
       </c>
-      <c r="C33" s="11">
-        <f>C14/demography!C3*100000</f>
+      <c r="C34">
+        <v>65662656</v>
+      </c>
+      <c r="D34" s="10">
+        <f>C14/C34*100000</f>
         <v>33.504584401824992</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>55</v>
+      <c r="E34" s="9">
+        <f>C16/C34*100000</f>
+        <v>22.844034819426131</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="9" t="s">
-        <v>56</v>
+      <c r="F34" s="9">
+        <f>C15/C34*100000</f>
+        <v>45.688069638852262</v>
       </c>
-      <c r="B34">
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35">
         <v>2020</v>
       </c>
-      <c r="C34" s="11">
-        <f>C5/demography!C4*100000</f>
+      <c r="C35">
+        <v>74292088</v>
+      </c>
+      <c r="D35" s="10">
+        <f>C5/C35*100000</f>
         <v>13.46038356062896</v>
       </c>
-      <c r="D34" s="9" t="s">
-        <v>55</v>
+      <c r="E35" s="9">
+        <f>C7/C35*100000</f>
+        <v>8.8838531500151134</v>
+      </c>
+      <c r="F35" s="9">
+        <f>C6/C35*100000</f>
+        <v>20.19057534094344</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="7"/>
+      <c r="C37" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>2000</v>
+      </c>
+      <c r="C38">
+        <v>78590624</v>
+      </c>
+      <c r="D38" s="10">
+        <f>C20/C38*100000</f>
+        <v>36.900076019246264</v>
+      </c>
+      <c r="E38" s="9">
+        <f>C25/C38*100000</f>
+        <v>25.448328289135354</v>
+      </c>
+      <c r="F38" s="9">
+        <f>C24/C38*100000</f>
+        <v>59.803571479468083</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>2010</v>
+      </c>
+      <c r="C39">
+        <v>86944961</v>
+      </c>
+      <c r="D39" s="10">
+        <f>C14/C39*100000</f>
+        <v>25.303364044294646</v>
+      </c>
+      <c r="E39" s="9">
+        <f>C16/C39*100000</f>
+        <v>17.25229366656453</v>
+      </c>
+      <c r="F39" s="9">
+        <f>C15/C39*100000</f>
+        <v>34.504587333129059</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>2020</v>
+      </c>
+      <c r="C40">
+        <v>96203595</v>
+      </c>
+      <c r="D40" s="10">
+        <f>C5/C40*100000</f>
+        <v>10.39462194733991</v>
+      </c>
+      <c r="E40" s="9">
+        <f>C7/C40*100000</f>
+        <v>6.86045048524434</v>
+      </c>
+      <c r="F40" s="9">
+        <f>C6/C40*100000</f>
+        <v>15.591932921009866</v>
       </c>
     </row>
   </sheetData>
@@ -30095,407 +30062,8 @@
     <hyperlink ref="A30" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5">
-        <v>2020</v>
-      </c>
-      <c r="C2" s="5">
-        <v>172000</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2020</v>
-      </c>
-      <c r="C3" s="5">
-        <v>110000</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="5">
-        <v>2020</v>
-      </c>
-      <c r="C4" s="5">
-        <v>247000</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2">
-        <v>2000</v>
-      </c>
-      <c r="C2">
-        <v>53576592</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3">
-        <v>2010</v>
-      </c>
-      <c r="C3">
-        <v>65662656</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4">
-        <v>2020</v>
-      </c>
-      <c r="C4">
-        <v>74292088</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="37.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5">
-        <v>2011</v>
-      </c>
-      <c r="C2" s="5">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2011</v>
-      </c>
-      <c r="C3" s="5">
-        <v>23.3</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="33.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5">
-        <v>2020</v>
-      </c>
-      <c r="C2" s="5">
-        <v>250000</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2020</v>
-      </c>
-      <c r="C3" s="5">
-        <v>230000</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="5">
-        <v>2020</v>
-      </c>
-      <c r="C4" s="5">
-        <v>270000</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="5">
-        <v>2020</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2020</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="5">
-        <v>2020</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D34:E34" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MDR proportion in spreadsheet and script
</commit_message>
<xml_diff>
--- a/data/calibration.xlsx
+++ b/data/calibration.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aschwalbc/Documents/Research/ACF-VN/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B41DB6E-D1DB-1B48-8363-C0CA018117AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4616C3F1-A2D2-8F48-ACF6-CC27EE914DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37900" yWindow="500" windowWidth="37900" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="33200" windowHeight="21380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notifications" sheetId="1" r:id="rId1"/>
     <sheet name="mortality" sheetId="2" r:id="rId2"/>
+    <sheet name="mdr" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="62">
   <si>
     <t>variable_name</t>
   </si>
@@ -161,6 +162,66 @@
   <si>
     <t>notifications per 100k</t>
   </si>
+  <si>
+    <t>Viet Nam</t>
+  </si>
+  <si>
+    <t>VNM</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>iso3</t>
+  </si>
+  <si>
+    <t>e_rr_pct_new</t>
+  </si>
+  <si>
+    <t>e_rr_pct_new_lo</t>
+  </si>
+  <si>
+    <t>e_rr_pct_new_hi</t>
+  </si>
+  <si>
+    <t>e_inc_rr_num</t>
+  </si>
+  <si>
+    <t>e_inc_rr_num_lo</t>
+  </si>
+  <si>
+    <t>e_inc_rr_num_hi</t>
+  </si>
+  <si>
+    <t>e_inc_100k</t>
+  </si>
+  <si>
+    <t>e_inc_100k_lo</t>
+  </si>
+  <si>
+    <t>e_inc_100k_hi</t>
+  </si>
+  <si>
+    <t>e_inc_num</t>
+  </si>
+  <si>
+    <t>e_inc_num_lo</t>
+  </si>
+  <si>
+    <t>e_inc_num_hi</t>
+  </si>
+  <si>
+    <t>From ''WHO MDR/RR-TB burden estimates" in https://www.who.int/teams/global-tuberculosis-programme/data</t>
+  </si>
+  <si>
+    <t>prop_mdr</t>
+  </si>
+  <si>
+    <t>prop_mdr_lo</t>
+  </si>
+  <si>
+    <t>prop_mdr_hi</t>
+  </si>
 </sst>
 </file>
 
@@ -245,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -259,6 +320,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,8 +541,8 @@
   </sheetPr>
   <dimension ref="A1:AA993"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F19" sqref="A19:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -30066,4 +30128,549 @@
     <ignoredError sqref="D34:E34" formula="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8847BFE-DB8F-7045-B6FB-60B017863E41}">
+  <dimension ref="A1:O20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2">
+        <v>2015</v>
+      </c>
+      <c r="D2">
+        <v>3.6</v>
+      </c>
+      <c r="E2">
+        <v>3.4</v>
+      </c>
+      <c r="F2">
+        <v>3.8</v>
+      </c>
+      <c r="G2">
+        <v>8300</v>
+      </c>
+      <c r="H2">
+        <v>4400</v>
+      </c>
+      <c r="I2">
+        <v>12000</v>
+      </c>
+      <c r="J2">
+        <v>199</v>
+      </c>
+      <c r="K2">
+        <v>117</v>
+      </c>
+      <c r="L2">
+        <v>303</v>
+      </c>
+      <c r="M2">
+        <v>184000</v>
+      </c>
+      <c r="N2">
+        <v>108000</v>
+      </c>
+      <c r="O2">
+        <v>279000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <v>2016</v>
+      </c>
+      <c r="D3">
+        <v>3.7</v>
+      </c>
+      <c r="E3">
+        <v>3.5</v>
+      </c>
+      <c r="F3">
+        <v>3.9</v>
+      </c>
+      <c r="G3">
+        <v>8300</v>
+      </c>
+      <c r="H3">
+        <v>4500</v>
+      </c>
+      <c r="I3">
+        <v>12000</v>
+      </c>
+      <c r="J3">
+        <v>193</v>
+      </c>
+      <c r="K3">
+        <v>116</v>
+      </c>
+      <c r="L3">
+        <v>290</v>
+      </c>
+      <c r="M3">
+        <v>180000</v>
+      </c>
+      <c r="N3">
+        <v>108000</v>
+      </c>
+      <c r="O3">
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>2017</v>
+      </c>
+      <c r="D4">
+        <v>3.8</v>
+      </c>
+      <c r="E4">
+        <v>3.7</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>8400</v>
+      </c>
+      <c r="H4">
+        <v>4700</v>
+      </c>
+      <c r="I4">
+        <v>12000</v>
+      </c>
+      <c r="J4">
+        <v>188</v>
+      </c>
+      <c r="K4">
+        <v>115</v>
+      </c>
+      <c r="L4">
+        <v>278</v>
+      </c>
+      <c r="M4">
+        <v>177000</v>
+      </c>
+      <c r="N4">
+        <v>108000</v>
+      </c>
+      <c r="O4">
+        <v>261000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>2018</v>
+      </c>
+      <c r="D5">
+        <v>3.9</v>
+      </c>
+      <c r="E5">
+        <v>3.8</v>
+      </c>
+      <c r="F5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G5">
+        <v>8400</v>
+      </c>
+      <c r="H5">
+        <v>4900</v>
+      </c>
+      <c r="I5">
+        <v>12000</v>
+      </c>
+      <c r="J5">
+        <v>182</v>
+      </c>
+      <c r="K5">
+        <v>114</v>
+      </c>
+      <c r="L5">
+        <v>265</v>
+      </c>
+      <c r="M5">
+        <v>173000</v>
+      </c>
+      <c r="N5">
+        <v>108000</v>
+      </c>
+      <c r="O5">
+        <v>252000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6">
+        <v>2019</v>
+      </c>
+      <c r="D6">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>4.2</v>
+      </c>
+      <c r="G6">
+        <v>8400</v>
+      </c>
+      <c r="H6">
+        <v>5000</v>
+      </c>
+      <c r="I6">
+        <v>12000</v>
+      </c>
+      <c r="J6">
+        <v>176</v>
+      </c>
+      <c r="K6">
+        <v>112</v>
+      </c>
+      <c r="L6">
+        <v>255</v>
+      </c>
+      <c r="M6">
+        <v>169000</v>
+      </c>
+      <c r="N6">
+        <v>108000</v>
+      </c>
+      <c r="O6">
+        <v>244000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7">
+        <v>2020</v>
+      </c>
+      <c r="D7">
+        <v>4.2</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>4.3</v>
+      </c>
+      <c r="G7">
+        <v>8500</v>
+      </c>
+      <c r="H7">
+        <v>5100</v>
+      </c>
+      <c r="I7">
+        <v>12000</v>
+      </c>
+      <c r="J7">
+        <v>171</v>
+      </c>
+      <c r="K7">
+        <v>110</v>
+      </c>
+      <c r="L7">
+        <v>244</v>
+      </c>
+      <c r="M7">
+        <v>165000</v>
+      </c>
+      <c r="N7">
+        <v>106000</v>
+      </c>
+      <c r="O7">
+        <v>236000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8">
+        <v>2021</v>
+      </c>
+      <c r="D8">
+        <v>4.3</v>
+      </c>
+      <c r="E8">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F8">
+        <v>4.5</v>
+      </c>
+      <c r="G8">
+        <v>8900</v>
+      </c>
+      <c r="H8">
+        <v>5400</v>
+      </c>
+      <c r="I8">
+        <v>12000</v>
+      </c>
+      <c r="J8">
+        <v>173</v>
+      </c>
+      <c r="K8">
+        <v>112</v>
+      </c>
+      <c r="L8">
+        <v>247</v>
+      </c>
+      <c r="M8">
+        <v>169000</v>
+      </c>
+      <c r="N8">
+        <v>109000</v>
+      </c>
+      <c r="O8">
+        <v>241000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>2015</v>
+      </c>
+      <c r="B13">
+        <f>G2/M2</f>
+        <v>4.5108695652173916E-2</v>
+      </c>
+      <c r="C13">
+        <f>H2/N2</f>
+        <v>4.0740740740740744E-2</v>
+      </c>
+      <c r="D13">
+        <f>I2/O2</f>
+        <v>4.3010752688172046E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>2016</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:B19" si="0">G3/M3</f>
+        <v>4.611111111111111E-2</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:C19" si="1">H3/N3</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D19" si="2">I3/O3</f>
+        <v>4.4444444444444446E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>2017</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>4.7457627118644069E-2</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>4.3518518518518519E-2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>4.5977011494252873E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>2018</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>4.8554913294797684E-2</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>4.5370370370370373E-2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>4.7619047619047616E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>2019</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>4.9704142011834318E-2</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>4.6296296296296294E-2</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>4.9180327868852458E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>2020</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>5.1515151515151514E-2</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>4.8113207547169815E-2</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>5.0847457627118647E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>2021</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>5.2662721893491124E-2</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>4.9541284403669728E-2</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>4.9792531120331947E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B20" s="11">
+        <f>AVERAGE(B13:B19)</f>
+        <v>4.8730623228171968E-2</v>
+      </c>
+      <c r="C20" s="11">
+        <f t="shared" ref="C20:D20" si="3">AVERAGE(C13:C19)</f>
+        <v>4.5035297791918873E-2</v>
+      </c>
+      <c r="D20" s="11">
+        <f t="shared" si="3"/>
+        <v>4.7267367551745716E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to MDR confidence intervals
</commit_message>
<xml_diff>
--- a/data/calibration.xlsx
+++ b/data/calibration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aschwalbc/Documents/Research/ACF-VN/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4616C3F1-A2D2-8F48-ACF6-CC27EE914DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19062306-EE04-E948-BBC9-7AB41C2E48DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="33200" windowHeight="21380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,8 +227,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -320,7 +321,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -30135,10 +30136,13 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
@@ -30546,12 +30550,12 @@
         <v>4.5108695652173916E-2</v>
       </c>
       <c r="C13">
-        <f>H2/N2</f>
-        <v>4.0740740740740744E-2</v>
+        <f>H2/M2</f>
+        <v>2.391304347826087E-2</v>
       </c>
       <c r="D13">
-        <f>I2/O2</f>
-        <v>4.3010752688172046E-2</v>
+        <f>I2/M2</f>
+        <v>6.5217391304347824E-2</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
@@ -30563,12 +30567,12 @@
         <v>4.611111111111111E-2</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:C19" si="1">H3/N3</f>
-        <v>4.1666666666666664E-2</v>
+        <f t="shared" ref="C14:C19" si="1">H3/M3</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D19" si="2">I3/O3</f>
-        <v>4.4444444444444446E-2</v>
+        <f t="shared" ref="D14:D19" si="2">I3/M3</f>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
@@ -30581,11 +30585,11 @@
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>4.3518518518518519E-2</v>
+        <v>2.655367231638418E-2</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>4.5977011494252873E-2</v>
+        <v>6.7796610169491525E-2</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
@@ -30598,11 +30602,11 @@
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>4.5370370370370373E-2</v>
+        <v>2.8323699421965318E-2</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>4.7619047619047616E-2</v>
+        <v>6.9364161849710976E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
@@ -30615,11 +30619,11 @@
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>4.6296296296296294E-2</v>
+        <v>2.9585798816568046E-2</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>4.9180327868852458E-2</v>
+        <v>7.1005917159763315E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -30632,11 +30636,11 @@
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>4.8113207547169815E-2</v>
+        <v>3.090909090909091E-2</v>
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>5.0847457627118647E-2</v>
+        <v>7.2727272727272724E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
@@ -30649,11 +30653,11 @@
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>4.9541284403669728E-2</v>
+        <v>3.1952662721893489E-2</v>
       </c>
       <c r="D19">
         <f t="shared" si="2"/>
-        <v>4.9792531120331947E-2</v>
+        <v>7.1005917159763315E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
@@ -30663,14 +30667,17 @@
       </c>
       <c r="C20" s="11">
         <f t="shared" ref="C20:D20" si="3">AVERAGE(C13:C19)</f>
-        <v>4.5035297791918873E-2</v>
+        <v>2.8033995380594683E-2</v>
       </c>
       <c r="D20" s="11">
         <f t="shared" si="3"/>
-        <v>4.7267367551745716E-2</v>
+        <v>6.9111991005288059E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C13:C19" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>